<commit_message>
Add Consensus Economics inflation forecasts
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\automate-RUS-ADO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C7E71686-3620-4C64-9FD3-85F7AD585DFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68626D0-1046-4122-9B7D-20866F70D02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">data!$C$1:$C$48</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
   <si>
     <t>region</t>
   </si>
@@ -361,16 +371,25 @@
     <t>forecast_gdp_2step</t>
   </si>
   <si>
-    <t>November 6, 2020</t>
-  </si>
-  <si>
     <t>iso_code</t>
+  </si>
+  <si>
+    <t>forecast_inf_1step</t>
+  </si>
+  <si>
+    <t>forecast_inf_2step</t>
+  </si>
+  <si>
+    <t>forecast_inf_current</t>
+  </si>
+  <si>
+    <t>November 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3310,11 +3329,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,7 +3341,7 @@
     <col min="7" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -3333,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" t="s">
         <v>77</v>
@@ -3353,8 +3372,17 @@
       <c r="J1" t="s">
         <v>110</v>
       </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3374,8 +3402,29 @@
       <c r="F2" s="2">
         <v>512</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I2">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J2">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K2">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L2">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M2">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3395,8 +3444,29 @@
       <c r="F3" s="2">
         <v>911</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I3">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J3">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K3">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L3">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M3">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3416,8 +3486,29 @@
       <c r="F4" s="2">
         <v>912</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I4">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J4">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K4">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L4">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M4">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -3437,8 +3528,29 @@
       <c r="F5" s="2">
         <v>513</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I5">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J5">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K5">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L5">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M5">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -3458,8 +3570,29 @@
       <c r="F6" s="2">
         <v>514</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I6">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J6">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K6">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L6">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M6">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -3479,8 +3612,29 @@
       <c r="F7" s="2">
         <v>516</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I7">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J7">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K7">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L7">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M7">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -3500,8 +3654,29 @@
       <c r="F8" s="2">
         <v>522</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I8">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J8">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K8">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L8">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M8">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -3520,8 +3695,29 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I9">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J9">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K9">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L9">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M9">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -3541,8 +3737,29 @@
       <c r="F10" s="2">
         <v>819</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I10">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J10">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K10">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L10">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M10">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -3562,8 +3779,29 @@
       <c r="F11" s="2">
         <v>868</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I11">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J11">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K11">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L11">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M11">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -3583,8 +3821,29 @@
       <c r="F12" s="2">
         <v>915</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I12">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J12">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K12">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L12">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M12">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3604,8 +3863,29 @@
       <c r="F13" s="2">
         <v>532</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I13">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J13">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K13">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L13">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M13">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3625,8 +3905,29 @@
       <c r="F14" s="2">
         <v>534</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I14">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J14">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K14">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L14">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M14">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -3646,8 +3947,29 @@
       <c r="F15" s="2">
         <v>536</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I15">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J15">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K15">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L15">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M15">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -3667,8 +3989,29 @@
       <c r="F16" s="2">
         <v>916</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I16">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J16">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K16">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L16">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M16">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -3688,8 +4031,29 @@
       <c r="F17" s="2">
         <v>917</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I17">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J17">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K17">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L17">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M17">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -3709,8 +4073,29 @@
       <c r="F18" s="2">
         <v>826</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I18">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J18">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K18">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L18">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M18">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3730,8 +4115,29 @@
       <c r="F19" s="2">
         <v>542</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I19">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J19">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K19">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L19">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M19">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -3751,8 +4157,29 @@
       <c r="F20" s="2">
         <v>544</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I20">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J20">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K20">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L20">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M20">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -3772,8 +4199,29 @@
       <c r="F21" s="2">
         <v>548</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I21">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J21">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K21">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L21">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M21">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -3793,8 +4241,29 @@
       <c r="F22" s="2">
         <v>556</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I22">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J22">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K22">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L22">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M22">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -3814,8 +4283,29 @@
       <c r="F23" s="2">
         <v>948</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I23">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J23">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K23">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L23">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M23">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -3835,8 +4325,29 @@
       <c r="F24" s="2">
         <v>518</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I24">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J24">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K24">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L24">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M24">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -3855,8 +4366,29 @@
       <c r="F25" s="2">
         <v>0</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I25">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J25">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K25">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L25">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M25">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -3876,8 +4408,29 @@
       <c r="F26" s="2">
         <v>558</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I26">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J26">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K26">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L26">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M26">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3896,8 +4449,29 @@
       <c r="F27" s="2">
         <v>0</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I27">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J27">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K27">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L27">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M27">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3917,8 +4491,29 @@
       <c r="F28" s="2">
         <v>564</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I28">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J28">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K28">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L28">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M28">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -3938,8 +4533,29 @@
       <c r="F29" s="2">
         <v>565</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I29">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J29">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K29">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L29">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M29">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -3959,8 +4575,29 @@
       <c r="F30" s="2">
         <v>566</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I30">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J30">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K30">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L30">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M30">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -3980,8 +4617,29 @@
       <c r="F31" s="2">
         <v>853</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I31">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J31">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K31">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L31">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M31">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -4001,8 +4659,29 @@
       <c r="F32" s="2">
         <v>924</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I32">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J32">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K32">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L32">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M32">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -4022,8 +4701,29 @@
       <c r="F33" s="2">
         <v>867</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I33">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J33">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K33">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L33">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M33">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -4044,19 +4744,28 @@
         <v>922</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H34">
-        <v>-4.0209999999999999</v>
+        <v>-3.8519999999999999</v>
       </c>
       <c r="I34">
-        <v>2.887</v>
+        <v>3.0129999999999999</v>
       </c>
       <c r="J34">
-        <v>2.177</v>
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K34">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L34">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M34">
+        <v>3.5760000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -4076,8 +4785,29 @@
       <c r="F35" s="2">
         <v>862</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I35">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J35">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K35">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L35">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M35">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -4097,8 +4827,29 @@
       <c r="F36" s="2">
         <v>576</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I36">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J36">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K36">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L36">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M36">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -4118,8 +4869,29 @@
       <c r="F37" s="2">
         <v>813</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I37">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J37">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K37">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L37">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M37">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -4139,8 +4911,29 @@
       <c r="F38" s="2">
         <v>524</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I38">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J38">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K38">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L38">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M38">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -4160,8 +4953,29 @@
       <c r="F39" s="2">
         <v>923</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I39">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J39">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K39">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L39">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M39">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -4181,8 +4995,29 @@
       <c r="F40" s="2">
         <v>528</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I40">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J40">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K40">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L40">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M40">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -4202,8 +5037,29 @@
       <c r="F41" s="2">
         <v>578</v>
       </c>
+      <c r="G41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I41">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J41">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K41">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L41">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M41">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -4223,8 +5079,29 @@
       <c r="F42" s="2">
         <v>537</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I42">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J42">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K42">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L42">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M42">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -4244,8 +5121,29 @@
       <c r="F43" s="2">
         <v>925</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H43">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I43">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J43">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K43">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L43">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M43">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -4265,8 +5163,29 @@
       <c r="F44" s="2">
         <v>866</v>
       </c>
+      <c r="G44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I44">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J44">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K44">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L44">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M44">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>71</v>
       </c>
@@ -4286,8 +5205,29 @@
       <c r="F45" s="2">
         <v>869</v>
       </c>
+      <c r="G45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H45">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I45">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J45">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K45">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L45">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M45">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -4307,8 +5247,29 @@
       <c r="F46" s="2">
         <v>927</v>
       </c>
+      <c r="G46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H46">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I46">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J46">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K46">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L46">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M46">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -4328,8 +5289,29 @@
       <c r="F47" s="2">
         <v>846</v>
       </c>
+      <c r="G47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I47">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J47">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K47">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L47">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M47">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -4349,9 +5331,30 @@
       <c r="F48" s="2">
         <v>582</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48">
+        <v>-3.8519999999999999</v>
+      </c>
+      <c r="I48">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="J48">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="K48">
+        <v>3.9159999999999999</v>
+      </c>
+      <c r="L48">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="M48">
+        <v>3.5760000000000001</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C48"/>
+  <autoFilter ref="C1:C48" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add other Consensus Economics forecasts
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68626D0-1046-4122-9B7D-20866F70D02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C00C19-A5A3-4FCA-887D-572B552A7460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="120">
   <si>
     <t>region</t>
   </si>
@@ -368,22 +368,34 @@
     <t>forecast_gdp_1step</t>
   </si>
   <si>
-    <t>forecast_gdp_2step</t>
-  </si>
-  <si>
     <t>iso_code</t>
   </si>
   <si>
     <t>forecast_inf_1step</t>
   </si>
   <si>
-    <t>forecast_inf_2step</t>
-  </si>
-  <si>
     <t>forecast_inf_current</t>
   </si>
   <si>
     <t>November 2020</t>
+  </si>
+  <si>
+    <t>forecast_con_current</t>
+  </si>
+  <si>
+    <t>forecast_con_1step</t>
+  </si>
+  <si>
+    <t>forecast_inv_current</t>
+  </si>
+  <si>
+    <t>forecast_inv_1step</t>
+  </si>
+  <si>
+    <t>forecast_ip_current</t>
+  </si>
+  <si>
+    <t>forecast_ip_1step</t>
   </si>
 </sst>
 </file>
@@ -3330,10 +3342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H3" sqref="H3:Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,7 +3353,7 @@
     <col min="7" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -3352,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
         <v>77</v>
@@ -3370,19 +3382,31 @@
         <v>109</v>
       </c>
       <c r="J1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" t="s">
         <v>112</v>
       </c>
-      <c r="M1" t="s">
-        <v>113</v>
+      <c r="Q1" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3403,28 +3427,40 @@
         <v>512</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H2">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I2">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J2">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K2">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L2">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M2">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N2">
+        <v>-3.5</v>
+      </c>
+      <c r="O2">
+        <v>3.2</v>
+      </c>
+      <c r="P2">
+        <v>3.9</v>
+      </c>
+      <c r="Q2">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3445,28 +3481,40 @@
         <v>911</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H3">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I3">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J3">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K3">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L3">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M3">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N3">
+        <v>-3.5</v>
+      </c>
+      <c r="O3">
+        <v>3.2</v>
+      </c>
+      <c r="P3">
+        <v>3.9</v>
+      </c>
+      <c r="Q3">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3487,28 +3535,40 @@
         <v>912</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H4">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I4">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J4">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K4">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L4">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M4">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N4">
+        <v>-3.5</v>
+      </c>
+      <c r="O4">
+        <v>3.2</v>
+      </c>
+      <c r="P4">
+        <v>3.9</v>
+      </c>
+      <c r="Q4">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -3529,28 +3589,40 @@
         <v>513</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H5">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I5">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J5">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K5">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L5">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M5">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N5">
+        <v>-3.5</v>
+      </c>
+      <c r="O5">
+        <v>3.2</v>
+      </c>
+      <c r="P5">
+        <v>3.9</v>
+      </c>
+      <c r="Q5">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -3571,28 +3643,40 @@
         <v>514</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H6">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I6">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J6">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K6">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L6">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M6">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N6">
+        <v>-3.5</v>
+      </c>
+      <c r="O6">
+        <v>3.2</v>
+      </c>
+      <c r="P6">
+        <v>3.9</v>
+      </c>
+      <c r="Q6">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -3613,28 +3697,40 @@
         <v>516</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H7">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I7">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J7">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K7">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L7">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M7">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N7">
+        <v>-3.5</v>
+      </c>
+      <c r="O7">
+        <v>3.2</v>
+      </c>
+      <c r="P7">
+        <v>3.9</v>
+      </c>
+      <c r="Q7">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -3655,28 +3751,40 @@
         <v>522</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H8">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I8">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J8">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K8">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L8">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M8">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N8">
+        <v>-3.5</v>
+      </c>
+      <c r="O8">
+        <v>3.2</v>
+      </c>
+      <c r="P8">
+        <v>3.9</v>
+      </c>
+      <c r="Q8">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -3696,28 +3804,40 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H9">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I9">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J9">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K9">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L9">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M9">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N9">
+        <v>-3.5</v>
+      </c>
+      <c r="O9">
+        <v>3.2</v>
+      </c>
+      <c r="P9">
+        <v>3.9</v>
+      </c>
+      <c r="Q9">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -3738,28 +3858,40 @@
         <v>819</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H10">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I10">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J10">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K10">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L10">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M10">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N10">
+        <v>-3.5</v>
+      </c>
+      <c r="O10">
+        <v>3.2</v>
+      </c>
+      <c r="P10">
+        <v>3.9</v>
+      </c>
+      <c r="Q10">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -3780,28 +3912,40 @@
         <v>868</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H11">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I11">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J11">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K11">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L11">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M11">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N11">
+        <v>-3.5</v>
+      </c>
+      <c r="O11">
+        <v>3.2</v>
+      </c>
+      <c r="P11">
+        <v>3.9</v>
+      </c>
+      <c r="Q11">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -3822,28 +3966,40 @@
         <v>915</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H12">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I12">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J12">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K12">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L12">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M12">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N12">
+        <v>-3.5</v>
+      </c>
+      <c r="O12">
+        <v>3.2</v>
+      </c>
+      <c r="P12">
+        <v>3.9</v>
+      </c>
+      <c r="Q12">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3864,28 +4020,40 @@
         <v>532</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H13">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I13">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J13">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K13">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L13">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M13">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N13">
+        <v>-3.5</v>
+      </c>
+      <c r="O13">
+        <v>3.2</v>
+      </c>
+      <c r="P13">
+        <v>3.9</v>
+      </c>
+      <c r="Q13">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3906,28 +4074,40 @@
         <v>534</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H14">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I14">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J14">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K14">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L14">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M14">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N14">
+        <v>-3.5</v>
+      </c>
+      <c r="O14">
+        <v>3.2</v>
+      </c>
+      <c r="P14">
+        <v>3.9</v>
+      </c>
+      <c r="Q14">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -3948,28 +4128,40 @@
         <v>536</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H15">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I15">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J15">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K15">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L15">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M15">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N15">
+        <v>-3.5</v>
+      </c>
+      <c r="O15">
+        <v>3.2</v>
+      </c>
+      <c r="P15">
+        <v>3.9</v>
+      </c>
+      <c r="Q15">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -3990,28 +4182,40 @@
         <v>916</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H16">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I16">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J16">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K16">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L16">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M16">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N16">
+        <v>-3.5</v>
+      </c>
+      <c r="O16">
+        <v>3.2</v>
+      </c>
+      <c r="P16">
+        <v>3.9</v>
+      </c>
+      <c r="Q16">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -4032,28 +4236,40 @@
         <v>917</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H17">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I17">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J17">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K17">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L17">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M17">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N17">
+        <v>-3.5</v>
+      </c>
+      <c r="O17">
+        <v>3.2</v>
+      </c>
+      <c r="P17">
+        <v>3.9</v>
+      </c>
+      <c r="Q17">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -4074,28 +4290,40 @@
         <v>826</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H18">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I18">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J18">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K18">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L18">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M18">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N18">
+        <v>-3.5</v>
+      </c>
+      <c r="O18">
+        <v>3.2</v>
+      </c>
+      <c r="P18">
+        <v>3.9</v>
+      </c>
+      <c r="Q18">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -4116,28 +4344,40 @@
         <v>542</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H19">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I19">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J19">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K19">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L19">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M19">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N19">
+        <v>-3.5</v>
+      </c>
+      <c r="O19">
+        <v>3.2</v>
+      </c>
+      <c r="P19">
+        <v>3.9</v>
+      </c>
+      <c r="Q19">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -4158,28 +4398,40 @@
         <v>544</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H20">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I20">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J20">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K20">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L20">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M20">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N20">
+        <v>-3.5</v>
+      </c>
+      <c r="O20">
+        <v>3.2</v>
+      </c>
+      <c r="P20">
+        <v>3.9</v>
+      </c>
+      <c r="Q20">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -4200,28 +4452,40 @@
         <v>548</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H21">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I21">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J21">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K21">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L21">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M21">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N21">
+        <v>-3.5</v>
+      </c>
+      <c r="O21">
+        <v>3.2</v>
+      </c>
+      <c r="P21">
+        <v>3.9</v>
+      </c>
+      <c r="Q21">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -4242,28 +4506,40 @@
         <v>556</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H22">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I22">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J22">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K22">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L22">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M22">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N22">
+        <v>-3.5</v>
+      </c>
+      <c r="O22">
+        <v>3.2</v>
+      </c>
+      <c r="P22">
+        <v>3.9</v>
+      </c>
+      <c r="Q22">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -4284,28 +4560,40 @@
         <v>948</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H23">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I23">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J23">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K23">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L23">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M23">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N23">
+        <v>-3.5</v>
+      </c>
+      <c r="O23">
+        <v>3.2</v>
+      </c>
+      <c r="P23">
+        <v>3.9</v>
+      </c>
+      <c r="Q23">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -4326,28 +4614,40 @@
         <v>518</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H24">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I24">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J24">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K24">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L24">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M24">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N24">
+        <v>-3.5</v>
+      </c>
+      <c r="O24">
+        <v>3.2</v>
+      </c>
+      <c r="P24">
+        <v>3.9</v>
+      </c>
+      <c r="Q24">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -4367,28 +4667,40 @@
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H25">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I25">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J25">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K25">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L25">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M25">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N25">
+        <v>-3.5</v>
+      </c>
+      <c r="O25">
+        <v>3.2</v>
+      </c>
+      <c r="P25">
+        <v>3.9</v>
+      </c>
+      <c r="Q25">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -4409,28 +4721,40 @@
         <v>558</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H26">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I26">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J26">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K26">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L26">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M26">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N26">
+        <v>-3.5</v>
+      </c>
+      <c r="O26">
+        <v>3.2</v>
+      </c>
+      <c r="P26">
+        <v>3.9</v>
+      </c>
+      <c r="Q26">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -4450,28 +4774,40 @@
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H27">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I27">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J27">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K27">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L27">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M27">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N27">
+        <v>-3.5</v>
+      </c>
+      <c r="O27">
+        <v>3.2</v>
+      </c>
+      <c r="P27">
+        <v>3.9</v>
+      </c>
+      <c r="Q27">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4492,28 +4828,40 @@
         <v>564</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H28">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I28">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J28">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K28">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L28">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M28">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N28">
+        <v>-3.5</v>
+      </c>
+      <c r="O28">
+        <v>3.2</v>
+      </c>
+      <c r="P28">
+        <v>3.9</v>
+      </c>
+      <c r="Q28">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -4534,28 +4882,40 @@
         <v>565</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H29">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I29">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J29">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K29">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L29">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M29">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N29">
+        <v>-3.5</v>
+      </c>
+      <c r="O29">
+        <v>3.2</v>
+      </c>
+      <c r="P29">
+        <v>3.9</v>
+      </c>
+      <c r="Q29">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -4576,28 +4936,40 @@
         <v>566</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H30">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I30">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J30">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K30">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L30">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M30">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N30">
+        <v>-3.5</v>
+      </c>
+      <c r="O30">
+        <v>3.2</v>
+      </c>
+      <c r="P30">
+        <v>3.9</v>
+      </c>
+      <c r="Q30">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -4618,28 +4990,40 @@
         <v>853</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H31">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I31">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J31">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K31">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L31">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M31">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N31">
+        <v>-3.5</v>
+      </c>
+      <c r="O31">
+        <v>3.2</v>
+      </c>
+      <c r="P31">
+        <v>3.9</v>
+      </c>
+      <c r="Q31">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -4660,28 +5044,40 @@
         <v>924</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H32">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I32">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J32">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K32">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L32">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M32">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N32">
+        <v>-3.5</v>
+      </c>
+      <c r="O32">
+        <v>3.2</v>
+      </c>
+      <c r="P32">
+        <v>3.9</v>
+      </c>
+      <c r="Q32">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -4702,28 +5098,40 @@
         <v>867</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H33">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I33">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J33">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K33">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L33">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M33">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N33">
+        <v>-3.5</v>
+      </c>
+      <c r="O33">
+        <v>3.2</v>
+      </c>
+      <c r="P33">
+        <v>3.9</v>
+      </c>
+      <c r="Q33">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -4744,28 +5152,40 @@
         <v>922</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H34">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I34">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J34">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K34">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L34">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M34">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N34">
+        <v>-3.5</v>
+      </c>
+      <c r="O34">
+        <v>3.2</v>
+      </c>
+      <c r="P34">
+        <v>3.9</v>
+      </c>
+      <c r="Q34">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -4786,28 +5206,40 @@
         <v>862</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H35">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I35">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J35">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K35">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L35">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M35">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N35">
+        <v>-3.5</v>
+      </c>
+      <c r="O35">
+        <v>3.2</v>
+      </c>
+      <c r="P35">
+        <v>3.9</v>
+      </c>
+      <c r="Q35">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -4828,28 +5260,40 @@
         <v>576</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H36">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I36">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J36">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K36">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L36">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M36">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N36">
+        <v>-3.5</v>
+      </c>
+      <c r="O36">
+        <v>3.2</v>
+      </c>
+      <c r="P36">
+        <v>3.9</v>
+      </c>
+      <c r="Q36">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -4870,28 +5314,40 @@
         <v>813</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H37">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I37">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J37">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K37">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L37">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M37">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N37">
+        <v>-3.5</v>
+      </c>
+      <c r="O37">
+        <v>3.2</v>
+      </c>
+      <c r="P37">
+        <v>3.9</v>
+      </c>
+      <c r="Q37">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -4912,28 +5368,40 @@
         <v>524</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H38">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I38">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J38">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K38">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L38">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M38">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N38">
+        <v>-3.5</v>
+      </c>
+      <c r="O38">
+        <v>3.2</v>
+      </c>
+      <c r="P38">
+        <v>3.9</v>
+      </c>
+      <c r="Q38">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -4954,28 +5422,40 @@
         <v>923</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H39">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I39">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J39">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K39">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L39">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M39">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N39">
+        <v>-3.5</v>
+      </c>
+      <c r="O39">
+        <v>3.2</v>
+      </c>
+      <c r="P39">
+        <v>3.9</v>
+      </c>
+      <c r="Q39">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -4996,28 +5476,40 @@
         <v>528</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H40">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I40">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J40">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K40">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L40">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M40">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N40">
+        <v>-3.5</v>
+      </c>
+      <c r="O40">
+        <v>3.2</v>
+      </c>
+      <c r="P40">
+        <v>3.9</v>
+      </c>
+      <c r="Q40">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -5038,28 +5530,40 @@
         <v>578</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H41">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I41">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J41">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K41">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L41">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M41">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N41">
+        <v>-3.5</v>
+      </c>
+      <c r="O41">
+        <v>3.2</v>
+      </c>
+      <c r="P41">
+        <v>3.9</v>
+      </c>
+      <c r="Q41">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5080,28 +5584,40 @@
         <v>537</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H42">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I42">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J42">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K42">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L42">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M42">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N42">
+        <v>-3.5</v>
+      </c>
+      <c r="O42">
+        <v>3.2</v>
+      </c>
+      <c r="P42">
+        <v>3.9</v>
+      </c>
+      <c r="Q42">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -5122,28 +5638,40 @@
         <v>925</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H43">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I43">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J43">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K43">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L43">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M43">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N43">
+        <v>-3.5</v>
+      </c>
+      <c r="O43">
+        <v>3.2</v>
+      </c>
+      <c r="P43">
+        <v>3.9</v>
+      </c>
+      <c r="Q43">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -5164,28 +5692,40 @@
         <v>866</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H44">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I44">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J44">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K44">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L44">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M44">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N44">
+        <v>-3.5</v>
+      </c>
+      <c r="O44">
+        <v>3.2</v>
+      </c>
+      <c r="P44">
+        <v>3.9</v>
+      </c>
+      <c r="Q44">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>71</v>
       </c>
@@ -5206,28 +5746,40 @@
         <v>869</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H45">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I45">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J45">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K45">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L45">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M45">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N45">
+        <v>-3.5</v>
+      </c>
+      <c r="O45">
+        <v>3.2</v>
+      </c>
+      <c r="P45">
+        <v>3.9</v>
+      </c>
+      <c r="Q45">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -5248,28 +5800,40 @@
         <v>927</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H46">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I46">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J46">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K46">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L46">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M46">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N46">
+        <v>-3.5</v>
+      </c>
+      <c r="O46">
+        <v>3.2</v>
+      </c>
+      <c r="P46">
+        <v>3.9</v>
+      </c>
+      <c r="Q46">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -5290,28 +5854,40 @@
         <v>846</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H47">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I47">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J47">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K47">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L47">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M47">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N47">
+        <v>-3.5</v>
+      </c>
+      <c r="O47">
+        <v>3.2</v>
+      </c>
+      <c r="P47">
+        <v>3.9</v>
+      </c>
+      <c r="Q47">
+        <v>3.6</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -5332,25 +5908,37 @@
         <v>582</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H48">
-        <v>-3.8519999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="I48">
-        <v>3.0129999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="J48">
-        <v>2.3340000000000001</v>
+        <v>-6.5</v>
       </c>
       <c r="K48">
-        <v>3.9159999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="L48">
-        <v>3.5950000000000002</v>
+        <v>-7.8</v>
       </c>
       <c r="M48">
-        <v>3.5760000000000001</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N48">
+        <v>-3.5</v>
+      </c>
+      <c r="O48">
+        <v>3.2</v>
+      </c>
+      <c r="P48">
+        <v>3.9</v>
+      </c>
+      <c r="Q48">
+        <v>3.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs for Russia
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C00C19-A5A3-4FCA-887D-572B552A7460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26CC997-D8CD-4E16-B2AB-46EDCB2E5358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3345,7 +3345,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:Q48"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3484,34 +3484,22 @@
         <v>113</v>
       </c>
       <c r="H3">
-        <v>-3.8</v>
+        <v>-5.7</v>
       </c>
       <c r="I3">
-        <v>3.1</v>
-      </c>
-      <c r="J3">
-        <v>-6.5</v>
-      </c>
-      <c r="K3">
-        <v>3.8</v>
-      </c>
-      <c r="L3">
-        <v>-7.8</v>
-      </c>
-      <c r="M3">
-        <v>4.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N3">
-        <v>-3.5</v>
+        <v>-5.7</v>
       </c>
       <c r="O3">
-        <v>3.2</v>
+        <v>6.2</v>
       </c>
       <c r="P3">
-        <v>3.9</v>
+        <v>0.9</v>
       </c>
       <c r="Q3">
-        <v>3.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Restructure output document and code
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26CC997-D8CD-4E16-B2AB-46EDCB2E5358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB3B735-245C-4253-A0A4-35409909F387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">data!$C$1:$C$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$C$1:$C$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -377,9 +377,6 @@
     <t>forecast_inf_current</t>
   </si>
   <si>
-    <t>November 2020</t>
-  </si>
-  <si>
     <t>forecast_con_current</t>
   </si>
   <si>
@@ -396,13 +393,19 @@
   </si>
   <si>
     <t>forecast_ip_1step</t>
+  </si>
+  <si>
+    <t>January 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +536,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -879,10 +888,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3345,7 +3355,10 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,22 +3395,22 @@
         <v>109</v>
       </c>
       <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
         <v>114</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>115</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>116</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>117</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>118</v>
-      </c>
-      <c r="O1" t="s">
-        <v>119</v>
       </c>
       <c r="P1" t="s">
         <v>112</v>
@@ -3427,37 +3440,37 @@
         <v>512</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2">
-        <v>-3.8</v>
-      </c>
-      <c r="I2">
-        <v>3.1</v>
-      </c>
-      <c r="J2">
-        <v>-6.5</v>
-      </c>
-      <c r="K2">
+        <v>119</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J2" s="3">
         <v>3.8</v>
       </c>
-      <c r="L2">
-        <v>-7.8</v>
-      </c>
-      <c r="M2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N2">
-        <v>-3.5</v>
-      </c>
-      <c r="O2">
-        <v>3.2</v>
-      </c>
-      <c r="P2">
-        <v>3.9</v>
-      </c>
-      <c r="Q2">
-        <v>3.6</v>
+      <c r="K2" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L2" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M2" s="3">
+        <v>4</v>
+      </c>
+      <c r="N2" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O2" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P2" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3481,25 +3494,37 @@
         <v>911</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3">
-        <v>-5.7</v>
-      </c>
-      <c r="I3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="N3">
-        <v>-5.7</v>
-      </c>
-      <c r="O3">
-        <v>6.2</v>
-      </c>
-      <c r="P3">
-        <v>0.9</v>
-      </c>
-      <c r="Q3">
-        <v>1.8</v>
+        <v>119</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M3" s="3">
+        <v>4</v>
+      </c>
+      <c r="N3" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O3" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P3" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -3523,37 +3548,37 @@
         <v>912</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H4">
-        <v>-3.8</v>
-      </c>
-      <c r="I4">
-        <v>3.1</v>
-      </c>
-      <c r="J4">
-        <v>-6.5</v>
-      </c>
-      <c r="K4">
+        <v>119</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J4" s="3">
         <v>3.8</v>
       </c>
-      <c r="L4">
-        <v>-7.8</v>
-      </c>
-      <c r="M4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N4">
-        <v>-3.5</v>
-      </c>
-      <c r="O4">
-        <v>3.2</v>
-      </c>
-      <c r="P4">
-        <v>3.9</v>
-      </c>
-      <c r="Q4">
-        <v>3.6</v>
+      <c r="K4" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M4" s="3">
+        <v>4</v>
+      </c>
+      <c r="N4" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3577,37 +3602,37 @@
         <v>513</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H5">
-        <v>-3.8</v>
-      </c>
-      <c r="I5">
-        <v>3.1</v>
-      </c>
-      <c r="J5">
-        <v>-6.5</v>
-      </c>
-      <c r="K5">
+        <v>119</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J5" s="3">
         <v>3.8</v>
       </c>
-      <c r="L5">
-        <v>-7.8</v>
-      </c>
-      <c r="M5">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N5">
-        <v>-3.5</v>
-      </c>
-      <c r="O5">
-        <v>3.2</v>
-      </c>
-      <c r="P5">
-        <v>3.9</v>
-      </c>
-      <c r="Q5">
-        <v>3.6</v>
+      <c r="K5" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>4</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P5" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -3631,37 +3656,37 @@
         <v>514</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6">
-        <v>-3.8</v>
-      </c>
-      <c r="I6">
-        <v>3.1</v>
-      </c>
-      <c r="J6">
-        <v>-6.5</v>
-      </c>
-      <c r="K6">
+        <v>119</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J6" s="3">
         <v>3.8</v>
       </c>
-      <c r="L6">
-        <v>-7.8</v>
-      </c>
-      <c r="M6">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N6">
-        <v>-3.5</v>
-      </c>
-      <c r="O6">
-        <v>3.2</v>
-      </c>
-      <c r="P6">
-        <v>3.9</v>
-      </c>
-      <c r="Q6">
-        <v>3.6</v>
+      <c r="K6" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M6" s="3">
+        <v>4</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P6" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -3685,38 +3710,18 @@
         <v>516</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7">
-        <v>-3.8</v>
-      </c>
-      <c r="I7">
-        <v>3.1</v>
-      </c>
-      <c r="J7">
-        <v>-6.5</v>
-      </c>
-      <c r="K7">
-        <v>3.8</v>
-      </c>
-      <c r="L7">
-        <v>-7.8</v>
-      </c>
-      <c r="M7">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N7">
-        <v>-3.5</v>
-      </c>
-      <c r="O7">
-        <v>3.2</v>
-      </c>
-      <c r="P7">
-        <v>3.9</v>
-      </c>
-      <c r="Q7">
-        <v>3.6</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3739,37 +3744,37 @@
         <v>522</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H8">
-        <v>-3.8</v>
-      </c>
-      <c r="I8">
-        <v>3.1</v>
-      </c>
-      <c r="J8">
-        <v>-6.5</v>
-      </c>
-      <c r="K8">
+        <v>119</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J8" s="3">
         <v>3.8</v>
       </c>
-      <c r="L8">
-        <v>-7.8</v>
-      </c>
-      <c r="M8">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N8">
-        <v>-3.5</v>
-      </c>
-      <c r="O8">
-        <v>3.2</v>
-      </c>
-      <c r="P8">
-        <v>3.9</v>
-      </c>
-      <c r="Q8">
-        <v>3.6</v>
+      <c r="K8" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M8" s="3">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O8" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3792,37 +3797,37 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9">
-        <v>-3.8</v>
-      </c>
-      <c r="I9">
-        <v>3.1</v>
-      </c>
-      <c r="J9">
-        <v>-6.5</v>
-      </c>
-      <c r="K9">
+        <v>119</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J9" s="3">
         <v>3.8</v>
       </c>
-      <c r="L9">
-        <v>-7.8</v>
-      </c>
-      <c r="M9">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N9">
-        <v>-3.5</v>
-      </c>
-      <c r="O9">
-        <v>3.2</v>
-      </c>
-      <c r="P9">
-        <v>3.9</v>
-      </c>
-      <c r="Q9">
-        <v>3.6</v>
+      <c r="K9" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L9" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M9" s="3">
+        <v>4</v>
+      </c>
+      <c r="N9" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O9" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P9" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3846,37 +3851,37 @@
         <v>819</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10">
-        <v>-3.8</v>
-      </c>
-      <c r="I10">
-        <v>3.1</v>
-      </c>
-      <c r="J10">
-        <v>-6.5</v>
-      </c>
-      <c r="K10">
+        <v>119</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J10" s="3">
         <v>3.8</v>
       </c>
-      <c r="L10">
-        <v>-7.8</v>
-      </c>
-      <c r="M10">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N10">
-        <v>-3.5</v>
-      </c>
-      <c r="O10">
-        <v>3.2</v>
-      </c>
-      <c r="P10">
-        <v>3.9</v>
-      </c>
-      <c r="Q10">
-        <v>3.6</v>
+      <c r="K10" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O10" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P10" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -3900,37 +3905,37 @@
         <v>868</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H11">
-        <v>-3.8</v>
-      </c>
-      <c r="I11">
-        <v>3.1</v>
-      </c>
-      <c r="J11">
-        <v>-6.5</v>
-      </c>
-      <c r="K11">
+        <v>119</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J11" s="3">
         <v>3.8</v>
       </c>
-      <c r="L11">
-        <v>-7.8</v>
-      </c>
-      <c r="M11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N11">
-        <v>-3.5</v>
-      </c>
-      <c r="O11">
-        <v>3.2</v>
-      </c>
-      <c r="P11">
-        <v>3.9</v>
-      </c>
-      <c r="Q11">
-        <v>3.6</v>
+      <c r="K11" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L11" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4</v>
+      </c>
+      <c r="N11" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O11" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P11" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -3954,37 +3959,37 @@
         <v>915</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12">
-        <v>-3.8</v>
-      </c>
-      <c r="I12">
-        <v>3.1</v>
-      </c>
-      <c r="J12">
-        <v>-6.5</v>
-      </c>
-      <c r="K12">
+        <v>119</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J12" s="3">
         <v>3.8</v>
       </c>
-      <c r="L12">
-        <v>-7.8</v>
-      </c>
-      <c r="M12">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N12">
-        <v>-3.5</v>
-      </c>
-      <c r="O12">
-        <v>3.2</v>
-      </c>
-      <c r="P12">
-        <v>3.9</v>
-      </c>
-      <c r="Q12">
-        <v>3.6</v>
+      <c r="K12" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>4</v>
+      </c>
+      <c r="N12" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O12" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P12" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -4008,37 +4013,37 @@
         <v>532</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13">
-        <v>-3.8</v>
-      </c>
-      <c r="I13">
-        <v>3.1</v>
-      </c>
-      <c r="J13">
-        <v>-6.5</v>
-      </c>
-      <c r="K13">
+        <v>119</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J13" s="3">
         <v>3.8</v>
       </c>
-      <c r="L13">
-        <v>-7.8</v>
-      </c>
-      <c r="M13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N13">
-        <v>-3.5</v>
-      </c>
-      <c r="O13">
-        <v>3.2</v>
-      </c>
-      <c r="P13">
-        <v>3.9</v>
-      </c>
-      <c r="Q13">
-        <v>3.6</v>
+      <c r="K13" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L13" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>4</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O13" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P13" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -4062,37 +4067,37 @@
         <v>534</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H14">
-        <v>-3.8</v>
-      </c>
-      <c r="I14">
-        <v>3.1</v>
-      </c>
-      <c r="J14">
-        <v>-6.5</v>
-      </c>
-      <c r="K14">
+        <v>119</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J14" s="3">
         <v>3.8</v>
       </c>
-      <c r="L14">
-        <v>-7.8</v>
-      </c>
-      <c r="M14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N14">
-        <v>-3.5</v>
-      </c>
-      <c r="O14">
-        <v>3.2</v>
-      </c>
-      <c r="P14">
-        <v>3.9</v>
-      </c>
-      <c r="Q14">
-        <v>3.6</v>
+      <c r="K14" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L14" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M14" s="3">
+        <v>4</v>
+      </c>
+      <c r="N14" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O14" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P14" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -4116,37 +4121,37 @@
         <v>536</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15">
-        <v>-3.8</v>
-      </c>
-      <c r="I15">
-        <v>3.1</v>
-      </c>
-      <c r="J15">
-        <v>-6.5</v>
-      </c>
-      <c r="K15">
+        <v>119</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J15" s="3">
         <v>3.8</v>
       </c>
-      <c r="L15">
-        <v>-7.8</v>
-      </c>
-      <c r="M15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N15">
-        <v>-3.5</v>
-      </c>
-      <c r="O15">
-        <v>3.2</v>
-      </c>
-      <c r="P15">
-        <v>3.9</v>
-      </c>
-      <c r="Q15">
-        <v>3.6</v>
+      <c r="K15" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L15" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M15" s="3">
+        <v>4</v>
+      </c>
+      <c r="N15" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O15" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P15" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4170,37 +4175,37 @@
         <v>916</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16">
-        <v>-3.8</v>
-      </c>
-      <c r="I16">
-        <v>3.1</v>
-      </c>
-      <c r="J16">
-        <v>-6.5</v>
-      </c>
-      <c r="K16">
+        <v>119</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J16" s="3">
         <v>3.8</v>
       </c>
-      <c r="L16">
-        <v>-7.8</v>
-      </c>
-      <c r="M16">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N16">
-        <v>-3.5</v>
-      </c>
-      <c r="O16">
-        <v>3.2</v>
-      </c>
-      <c r="P16">
-        <v>3.9</v>
-      </c>
-      <c r="Q16">
-        <v>3.6</v>
+      <c r="K16" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L16" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M16" s="3">
+        <v>4</v>
+      </c>
+      <c r="N16" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O16" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P16" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -4224,37 +4229,37 @@
         <v>917</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17">
-        <v>-3.8</v>
-      </c>
-      <c r="I17">
-        <v>3.1</v>
-      </c>
-      <c r="J17">
-        <v>-6.5</v>
-      </c>
-      <c r="K17">
+        <v>119</v>
+      </c>
+      <c r="H17" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J17" s="3">
         <v>3.8</v>
       </c>
-      <c r="L17">
-        <v>-7.8</v>
-      </c>
-      <c r="M17">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N17">
-        <v>-3.5</v>
-      </c>
-      <c r="O17">
-        <v>3.2</v>
-      </c>
-      <c r="P17">
-        <v>3.9</v>
-      </c>
-      <c r="Q17">
-        <v>3.6</v>
+      <c r="K17" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L17" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M17" s="3">
+        <v>4</v>
+      </c>
+      <c r="N17" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O17" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P17" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -4278,37 +4283,37 @@
         <v>826</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18">
-        <v>-3.8</v>
-      </c>
-      <c r="I18">
-        <v>3.1</v>
-      </c>
-      <c r="J18">
-        <v>-6.5</v>
-      </c>
-      <c r="K18">
+        <v>119</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J18" s="3">
         <v>3.8</v>
       </c>
-      <c r="L18">
-        <v>-7.8</v>
-      </c>
-      <c r="M18">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N18">
-        <v>-3.5</v>
-      </c>
-      <c r="O18">
-        <v>3.2</v>
-      </c>
-      <c r="P18">
-        <v>3.9</v>
-      </c>
-      <c r="Q18">
-        <v>3.6</v>
+      <c r="K18" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L18" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M18" s="3">
+        <v>4</v>
+      </c>
+      <c r="N18" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O18" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P18" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -4332,37 +4337,37 @@
         <v>542</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19">
-        <v>-3.8</v>
-      </c>
-      <c r="I19">
-        <v>3.1</v>
-      </c>
-      <c r="J19">
-        <v>-6.5</v>
-      </c>
-      <c r="K19">
+        <v>119</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J19" s="3">
         <v>3.8</v>
       </c>
-      <c r="L19">
-        <v>-7.8</v>
-      </c>
-      <c r="M19">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N19">
-        <v>-3.5</v>
-      </c>
-      <c r="O19">
-        <v>3.2</v>
-      </c>
-      <c r="P19">
-        <v>3.9</v>
-      </c>
-      <c r="Q19">
-        <v>3.6</v>
+      <c r="K19" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L19" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M19" s="3">
+        <v>4</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O19" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P19" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -4386,37 +4391,37 @@
         <v>544</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20">
-        <v>-3.8</v>
-      </c>
-      <c r="I20">
-        <v>3.1</v>
-      </c>
-      <c r="J20">
-        <v>-6.5</v>
-      </c>
-      <c r="K20">
+        <v>119</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J20" s="3">
         <v>3.8</v>
       </c>
-      <c r="L20">
-        <v>-7.8</v>
-      </c>
-      <c r="M20">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N20">
-        <v>-3.5</v>
-      </c>
-      <c r="O20">
-        <v>3.2</v>
-      </c>
-      <c r="P20">
-        <v>3.9</v>
-      </c>
-      <c r="Q20">
-        <v>3.6</v>
+      <c r="K20" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M20" s="3">
+        <v>4</v>
+      </c>
+      <c r="N20" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O20" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P20" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -4440,37 +4445,37 @@
         <v>548</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H21">
-        <v>-3.8</v>
-      </c>
-      <c r="I21">
-        <v>3.1</v>
-      </c>
-      <c r="J21">
-        <v>-6.5</v>
-      </c>
-      <c r="K21">
-        <v>3.8</v>
-      </c>
-      <c r="L21">
-        <v>-7.8</v>
-      </c>
-      <c r="M21">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N21">
-        <v>-3.5</v>
-      </c>
-      <c r="O21">
-        <v>3.2</v>
-      </c>
-      <c r="P21">
-        <v>3.9</v>
-      </c>
-      <c r="Q21">
-        <v>3.6</v>
+        <v>119</v>
+      </c>
+      <c r="H21" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I21" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="K21" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="L21" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M21" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="O21" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="P21" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -4494,37 +4499,37 @@
         <v>556</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22">
-        <v>-3.8</v>
-      </c>
-      <c r="I22">
-        <v>3.1</v>
-      </c>
-      <c r="J22">
-        <v>-6.5</v>
-      </c>
-      <c r="K22">
+        <v>119</v>
+      </c>
+      <c r="H22" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J22" s="3">
         <v>3.8</v>
       </c>
-      <c r="L22">
-        <v>-7.8</v>
-      </c>
-      <c r="M22">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N22">
-        <v>-3.5</v>
-      </c>
-      <c r="O22">
-        <v>3.2</v>
-      </c>
-      <c r="P22">
-        <v>3.9</v>
-      </c>
-      <c r="Q22">
-        <v>3.6</v>
+      <c r="K22" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>4</v>
+      </c>
+      <c r="N22" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O22" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P22" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -4548,37 +4553,37 @@
         <v>948</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23">
-        <v>-3.8</v>
-      </c>
-      <c r="I23">
-        <v>3.1</v>
-      </c>
-      <c r="J23">
-        <v>-6.5</v>
-      </c>
-      <c r="K23">
+        <v>119</v>
+      </c>
+      <c r="H23" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J23" s="3">
         <v>3.8</v>
       </c>
-      <c r="L23">
-        <v>-7.8</v>
-      </c>
-      <c r="M23">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N23">
-        <v>-3.5</v>
-      </c>
-      <c r="O23">
-        <v>3.2</v>
-      </c>
-      <c r="P23">
-        <v>3.9</v>
-      </c>
-      <c r="Q23">
-        <v>3.6</v>
+      <c r="K23" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4</v>
+      </c>
+      <c r="N23" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O23" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P23" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -4602,37 +4607,37 @@
         <v>518</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H24">
-        <v>-3.8</v>
-      </c>
-      <c r="I24">
-        <v>3.1</v>
-      </c>
-      <c r="J24">
-        <v>-6.5</v>
-      </c>
-      <c r="K24">
+        <v>119</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I24" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J24" s="3">
         <v>3.8</v>
       </c>
-      <c r="L24">
-        <v>-7.8</v>
-      </c>
-      <c r="M24">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N24">
-        <v>-3.5</v>
-      </c>
-      <c r="O24">
-        <v>3.2</v>
-      </c>
-      <c r="P24">
-        <v>3.9</v>
-      </c>
-      <c r="Q24">
-        <v>3.6</v>
+      <c r="K24" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L24" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>4</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O24" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P24" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -4655,37 +4660,37 @@
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H25">
-        <v>-3.8</v>
-      </c>
-      <c r="I25">
-        <v>3.1</v>
-      </c>
-      <c r="J25">
-        <v>-6.5</v>
-      </c>
-      <c r="K25">
+        <v>119</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I25" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J25" s="3">
         <v>3.8</v>
       </c>
-      <c r="L25">
-        <v>-7.8</v>
-      </c>
-      <c r="M25">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N25">
-        <v>-3.5</v>
-      </c>
-      <c r="O25">
-        <v>3.2</v>
-      </c>
-      <c r="P25">
-        <v>3.9</v>
-      </c>
-      <c r="Q25">
-        <v>3.6</v>
+      <c r="K25" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L25" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M25" s="3">
+        <v>4</v>
+      </c>
+      <c r="N25" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O25" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P25" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -4709,37 +4714,37 @@
         <v>558</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26">
-        <v>-3.8</v>
-      </c>
-      <c r="I26">
-        <v>3.1</v>
-      </c>
-      <c r="J26">
-        <v>-6.5</v>
-      </c>
-      <c r="K26">
+        <v>119</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J26" s="3">
         <v>3.8</v>
       </c>
-      <c r="L26">
-        <v>-7.8</v>
-      </c>
-      <c r="M26">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N26">
-        <v>-3.5</v>
-      </c>
-      <c r="O26">
-        <v>3.2</v>
-      </c>
-      <c r="P26">
-        <v>3.9</v>
-      </c>
-      <c r="Q26">
-        <v>3.6</v>
+      <c r="K26" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>4</v>
+      </c>
+      <c r="N26" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O26" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P26" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -4762,37 +4767,37 @@
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H27">
-        <v>-3.8</v>
-      </c>
-      <c r="I27">
-        <v>3.1</v>
-      </c>
-      <c r="J27">
-        <v>-6.5</v>
-      </c>
-      <c r="K27">
+        <v>119</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J27" s="3">
         <v>3.8</v>
       </c>
-      <c r="L27">
-        <v>-7.8</v>
-      </c>
-      <c r="M27">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N27">
-        <v>-3.5</v>
-      </c>
-      <c r="O27">
-        <v>3.2</v>
-      </c>
-      <c r="P27">
-        <v>3.9</v>
-      </c>
-      <c r="Q27">
-        <v>3.6</v>
+      <c r="K27" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L27" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M27" s="3">
+        <v>4</v>
+      </c>
+      <c r="N27" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O27" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P27" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -4816,37 +4821,37 @@
         <v>564</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H28">
-        <v>-3.8</v>
-      </c>
-      <c r="I28">
-        <v>3.1</v>
-      </c>
-      <c r="J28">
-        <v>-6.5</v>
-      </c>
-      <c r="K28">
+        <v>119</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J28" s="3">
         <v>3.8</v>
       </c>
-      <c r="L28">
-        <v>-7.8</v>
-      </c>
-      <c r="M28">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N28">
-        <v>-3.5</v>
-      </c>
-      <c r="O28">
-        <v>3.2</v>
-      </c>
-      <c r="P28">
-        <v>3.9</v>
-      </c>
-      <c r="Q28">
-        <v>3.6</v>
+      <c r="K28" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L28" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M28" s="3">
+        <v>4</v>
+      </c>
+      <c r="N28" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O28" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P28" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -4870,37 +4875,37 @@
         <v>565</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H29">
-        <v>-3.8</v>
-      </c>
-      <c r="I29">
-        <v>3.1</v>
-      </c>
-      <c r="J29">
-        <v>-6.5</v>
-      </c>
-      <c r="K29">
+        <v>119</v>
+      </c>
+      <c r="H29" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I29" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J29" s="3">
         <v>3.8</v>
       </c>
-      <c r="L29">
-        <v>-7.8</v>
-      </c>
-      <c r="M29">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N29">
-        <v>-3.5</v>
-      </c>
-      <c r="O29">
-        <v>3.2</v>
-      </c>
-      <c r="P29">
-        <v>3.9</v>
-      </c>
-      <c r="Q29">
-        <v>3.6</v>
+      <c r="K29" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L29" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M29" s="3">
+        <v>4</v>
+      </c>
+      <c r="N29" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O29" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P29" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -4924,37 +4929,37 @@
         <v>566</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H30">
-        <v>-3.8</v>
-      </c>
-      <c r="I30">
+        <v>119</v>
+      </c>
+      <c r="H30" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="I30" s="3">
+        <v>7</v>
+      </c>
+      <c r="J30" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="K30" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="L30" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="M30" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="N30" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="O30" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P30" s="3">
         <v>3.1</v>
       </c>
-      <c r="J30">
-        <v>-6.5</v>
-      </c>
-      <c r="K30">
-        <v>3.8</v>
-      </c>
-      <c r="L30">
-        <v>-7.8</v>
-      </c>
-      <c r="M30">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N30">
-        <v>-3.5</v>
-      </c>
-      <c r="O30">
-        <v>3.2</v>
-      </c>
-      <c r="P30">
-        <v>3.9</v>
-      </c>
-      <c r="Q30">
-        <v>3.6</v>
+      <c r="Q30" s="3">
+        <v>3.2</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -4978,37 +4983,37 @@
         <v>853</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H31">
-        <v>-3.8</v>
-      </c>
-      <c r="I31">
-        <v>3.1</v>
-      </c>
-      <c r="J31">
-        <v>-6.5</v>
-      </c>
-      <c r="K31">
+        <v>119</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J31" s="3">
         <v>3.8</v>
       </c>
-      <c r="L31">
-        <v>-7.8</v>
-      </c>
-      <c r="M31">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N31">
-        <v>-3.5</v>
-      </c>
-      <c r="O31">
-        <v>3.2</v>
-      </c>
-      <c r="P31">
-        <v>3.9</v>
-      </c>
-      <c r="Q31">
-        <v>3.6</v>
+      <c r="K31" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L31" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M31" s="3">
+        <v>4</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O31" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P31" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -5032,37 +5037,37 @@
         <v>924</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H32">
-        <v>-3.8</v>
-      </c>
-      <c r="I32">
-        <v>3.1</v>
-      </c>
-      <c r="J32">
-        <v>-6.5</v>
-      </c>
-      <c r="K32">
-        <v>3.8</v>
-      </c>
-      <c r="L32">
-        <v>-7.8</v>
-      </c>
-      <c r="M32">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N32">
-        <v>-3.5</v>
-      </c>
-      <c r="O32">
-        <v>3.2</v>
-      </c>
-      <c r="P32">
-        <v>3.9</v>
-      </c>
-      <c r="Q32">
-        <v>3.6</v>
+        <v>119</v>
+      </c>
+      <c r="H32" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I32" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="J32" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="K32" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="L32" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="M32" s="3">
+        <v>5</v>
+      </c>
+      <c r="N32" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="O32" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="P32" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>2.1</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -5086,37 +5091,37 @@
         <v>867</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H33">
-        <v>-3.8</v>
-      </c>
-      <c r="I33">
-        <v>3.1</v>
-      </c>
-      <c r="J33">
-        <v>-6.5</v>
-      </c>
-      <c r="K33">
+        <v>119</v>
+      </c>
+      <c r="H33" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I33" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J33" s="3">
         <v>3.8</v>
       </c>
-      <c r="L33">
-        <v>-7.8</v>
-      </c>
-      <c r="M33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N33">
-        <v>-3.5</v>
-      </c>
-      <c r="O33">
-        <v>3.2</v>
-      </c>
-      <c r="P33">
-        <v>3.9</v>
-      </c>
-      <c r="Q33">
-        <v>3.6</v>
+      <c r="K33" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L33" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M33" s="3">
+        <v>4</v>
+      </c>
+      <c r="N33" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O33" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P33" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -5140,37 +5145,37 @@
         <v>922</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H34">
-        <v>-3.8</v>
-      </c>
-      <c r="I34">
-        <v>3.1</v>
-      </c>
-      <c r="J34">
-        <v>-6.5</v>
-      </c>
-      <c r="K34">
+        <v>119</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J34" s="3">
         <v>3.8</v>
       </c>
-      <c r="L34">
-        <v>-7.8</v>
-      </c>
-      <c r="M34">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N34">
-        <v>-3.5</v>
-      </c>
-      <c r="O34">
-        <v>3.2</v>
-      </c>
-      <c r="P34">
-        <v>3.9</v>
-      </c>
-      <c r="Q34">
-        <v>3.6</v>
+      <c r="K34" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L34" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M34" s="3">
+        <v>4</v>
+      </c>
+      <c r="N34" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O34" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P34" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -5194,37 +5199,37 @@
         <v>862</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H35">
-        <v>-3.8</v>
-      </c>
-      <c r="I35">
-        <v>3.1</v>
-      </c>
-      <c r="J35">
-        <v>-6.5</v>
-      </c>
-      <c r="K35">
+        <v>119</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I35" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J35" s="3">
         <v>3.8</v>
       </c>
-      <c r="L35">
-        <v>-7.8</v>
-      </c>
-      <c r="M35">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N35">
-        <v>-3.5</v>
-      </c>
-      <c r="O35">
-        <v>3.2</v>
-      </c>
-      <c r="P35">
-        <v>3.9</v>
-      </c>
-      <c r="Q35">
-        <v>3.6</v>
+      <c r="K35" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L35" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M35" s="3">
+        <v>4</v>
+      </c>
+      <c r="N35" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O35" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P35" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -5248,37 +5253,37 @@
         <v>576</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H36">
-        <v>-3.8</v>
-      </c>
-      <c r="I36">
-        <v>3.1</v>
-      </c>
-      <c r="J36">
-        <v>-6.5</v>
-      </c>
-      <c r="K36">
-        <v>3.8</v>
-      </c>
-      <c r="L36">
-        <v>-7.8</v>
-      </c>
-      <c r="M36">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N36">
-        <v>-3.5</v>
-      </c>
-      <c r="O36">
-        <v>3.2</v>
-      </c>
-      <c r="P36">
-        <v>3.9</v>
-      </c>
-      <c r="Q36">
-        <v>3.6</v>
+        <v>119</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I36" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="J36" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K36" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="L36" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="M36" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="N36" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="O36" s="3">
+        <v>4</v>
+      </c>
+      <c r="P36" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>1.2</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -5302,37 +5307,37 @@
         <v>813</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H37">
-        <v>-3.8</v>
-      </c>
-      <c r="I37">
-        <v>3.1</v>
-      </c>
-      <c r="J37">
-        <v>-6.5</v>
-      </c>
-      <c r="K37">
+        <v>119</v>
+      </c>
+      <c r="H37" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I37" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J37" s="3">
         <v>3.8</v>
       </c>
-      <c r="L37">
-        <v>-7.8</v>
-      </c>
-      <c r="M37">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N37">
-        <v>-3.5</v>
-      </c>
-      <c r="O37">
-        <v>3.2</v>
-      </c>
-      <c r="P37">
-        <v>3.9</v>
-      </c>
-      <c r="Q37">
-        <v>3.6</v>
+      <c r="K37" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L37" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M37" s="3">
+        <v>4</v>
+      </c>
+      <c r="N37" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O37" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P37" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -5356,37 +5361,37 @@
         <v>524</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H38">
-        <v>-3.8</v>
-      </c>
-      <c r="I38">
-        <v>3.1</v>
-      </c>
-      <c r="J38">
-        <v>-6.5</v>
-      </c>
-      <c r="K38">
+        <v>119</v>
+      </c>
+      <c r="H38" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I38" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J38" s="3">
         <v>3.8</v>
       </c>
-      <c r="L38">
-        <v>-7.8</v>
-      </c>
-      <c r="M38">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N38">
-        <v>-3.5</v>
-      </c>
-      <c r="O38">
-        <v>3.2</v>
-      </c>
-      <c r="P38">
-        <v>3.9</v>
-      </c>
-      <c r="Q38">
-        <v>3.6</v>
+      <c r="K38" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L38" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M38" s="3">
+        <v>4</v>
+      </c>
+      <c r="N38" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O38" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P38" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -5410,37 +5415,37 @@
         <v>923</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H39">
-        <v>-3.8</v>
-      </c>
-      <c r="I39">
-        <v>3.1</v>
-      </c>
-      <c r="J39">
-        <v>-6.5</v>
-      </c>
-      <c r="K39">
+        <v>119</v>
+      </c>
+      <c r="H39" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I39" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J39" s="3">
         <v>3.8</v>
       </c>
-      <c r="L39">
-        <v>-7.8</v>
-      </c>
-      <c r="M39">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N39">
-        <v>-3.5</v>
-      </c>
-      <c r="O39">
-        <v>3.2</v>
-      </c>
-      <c r="P39">
-        <v>3.9</v>
-      </c>
-      <c r="Q39">
-        <v>3.6</v>
+      <c r="K39" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L39" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M39" s="3">
+        <v>4</v>
+      </c>
+      <c r="N39" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O39" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P39" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -5464,37 +5469,37 @@
         <v>528</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H40">
-        <v>-3.8</v>
-      </c>
-      <c r="I40">
+        <v>119</v>
+      </c>
+      <c r="H40" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I40" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="J40" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="K40" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L40" s="3">
         <v>3.1</v>
       </c>
-      <c r="J40">
-        <v>-6.5</v>
-      </c>
-      <c r="K40">
-        <v>3.8</v>
-      </c>
-      <c r="L40">
-        <v>-7.8</v>
-      </c>
-      <c r="M40">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N40">
-        <v>-3.5</v>
-      </c>
-      <c r="O40">
-        <v>3.2</v>
-      </c>
-      <c r="P40">
-        <v>3.9</v>
-      </c>
-      <c r="Q40">
-        <v>3.6</v>
+      <c r="M40" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="N40" s="3">
+        <v>6</v>
+      </c>
+      <c r="O40" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="P40" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>1.2</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -5518,37 +5523,37 @@
         <v>578</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H41">
-        <v>-3.8</v>
-      </c>
-      <c r="I41">
-        <v>3.1</v>
-      </c>
-      <c r="J41">
-        <v>-6.5</v>
-      </c>
-      <c r="K41">
+        <v>119</v>
+      </c>
+      <c r="H41" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J41" s="3">
         <v>3.8</v>
       </c>
-      <c r="L41">
-        <v>-7.8</v>
-      </c>
-      <c r="M41">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N41">
-        <v>-3.5</v>
-      </c>
-      <c r="O41">
-        <v>3.2</v>
-      </c>
-      <c r="P41">
-        <v>3.9</v>
-      </c>
-      <c r="Q41">
-        <v>3.6</v>
+      <c r="K41" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L41" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M41" s="3">
+        <v>4</v>
+      </c>
+      <c r="N41" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O41" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P41" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -5572,37 +5577,37 @@
         <v>537</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H42">
-        <v>-3.8</v>
-      </c>
-      <c r="I42">
-        <v>3.1</v>
-      </c>
-      <c r="J42">
-        <v>-6.5</v>
-      </c>
-      <c r="K42">
+        <v>119</v>
+      </c>
+      <c r="H42" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I42" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J42" s="3">
         <v>3.8</v>
       </c>
-      <c r="L42">
-        <v>-7.8</v>
-      </c>
-      <c r="M42">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N42">
-        <v>-3.5</v>
-      </c>
-      <c r="O42">
-        <v>3.2</v>
-      </c>
-      <c r="P42">
-        <v>3.9</v>
-      </c>
-      <c r="Q42">
-        <v>3.6</v>
+      <c r="K42" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L42" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M42" s="3">
+        <v>4</v>
+      </c>
+      <c r="N42" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O42" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P42" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -5626,37 +5631,37 @@
         <v>925</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H43">
-        <v>-3.8</v>
-      </c>
-      <c r="I43">
-        <v>3.1</v>
-      </c>
-      <c r="J43">
-        <v>-6.5</v>
-      </c>
-      <c r="K43">
+        <v>119</v>
+      </c>
+      <c r="H43" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I43" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J43" s="3">
         <v>3.8</v>
       </c>
-      <c r="L43">
-        <v>-7.8</v>
-      </c>
-      <c r="M43">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N43">
-        <v>-3.5</v>
-      </c>
-      <c r="O43">
-        <v>3.2</v>
-      </c>
-      <c r="P43">
-        <v>3.9</v>
-      </c>
-      <c r="Q43">
-        <v>3.6</v>
+      <c r="K43" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L43" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M43" s="3">
+        <v>4</v>
+      </c>
+      <c r="N43" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O43" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P43" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -5680,37 +5685,37 @@
         <v>866</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H44">
-        <v>-3.8</v>
-      </c>
-      <c r="I44">
-        <v>3.1</v>
-      </c>
-      <c r="J44">
-        <v>-6.5</v>
-      </c>
-      <c r="K44">
+        <v>119</v>
+      </c>
+      <c r="H44" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I44" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J44" s="3">
         <v>3.8</v>
       </c>
-      <c r="L44">
-        <v>-7.8</v>
-      </c>
-      <c r="M44">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N44">
-        <v>-3.5</v>
-      </c>
-      <c r="O44">
-        <v>3.2</v>
-      </c>
-      <c r="P44">
-        <v>3.9</v>
-      </c>
-      <c r="Q44">
-        <v>3.6</v>
+      <c r="K44" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L44" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M44" s="3">
+        <v>4</v>
+      </c>
+      <c r="N44" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O44" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P44" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -5734,37 +5739,37 @@
         <v>869</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H45">
-        <v>-3.8</v>
-      </c>
-      <c r="I45">
-        <v>3.1</v>
-      </c>
-      <c r="J45">
-        <v>-6.5</v>
-      </c>
-      <c r="K45">
+        <v>119</v>
+      </c>
+      <c r="H45" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I45" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J45" s="3">
         <v>3.8</v>
       </c>
-      <c r="L45">
-        <v>-7.8</v>
-      </c>
-      <c r="M45">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N45">
-        <v>-3.5</v>
-      </c>
-      <c r="O45">
-        <v>3.2</v>
-      </c>
-      <c r="P45">
-        <v>3.9</v>
-      </c>
-      <c r="Q45">
-        <v>3.6</v>
+      <c r="K45" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L45" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M45" s="3">
+        <v>4</v>
+      </c>
+      <c r="N45" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O45" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P45" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -5788,37 +5793,37 @@
         <v>927</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H46">
-        <v>-3.8</v>
-      </c>
-      <c r="I46">
-        <v>3.1</v>
-      </c>
-      <c r="J46">
-        <v>-6.5</v>
-      </c>
-      <c r="K46">
+        <v>119</v>
+      </c>
+      <c r="H46" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I46" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J46" s="3">
         <v>3.8</v>
       </c>
-      <c r="L46">
-        <v>-7.8</v>
-      </c>
-      <c r="M46">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N46">
-        <v>-3.5</v>
-      </c>
-      <c r="O46">
-        <v>3.2</v>
-      </c>
-      <c r="P46">
-        <v>3.9</v>
-      </c>
-      <c r="Q46">
-        <v>3.6</v>
+      <c r="K46" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L46" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M46" s="3">
+        <v>4</v>
+      </c>
+      <c r="N46" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O46" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P46" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -5842,37 +5847,37 @@
         <v>846</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H47">
-        <v>-3.8</v>
-      </c>
-      <c r="I47">
-        <v>3.1</v>
-      </c>
-      <c r="J47">
-        <v>-6.5</v>
-      </c>
-      <c r="K47">
+        <v>119</v>
+      </c>
+      <c r="H47" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I47" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J47" s="3">
         <v>3.8</v>
       </c>
-      <c r="L47">
-        <v>-7.8</v>
-      </c>
-      <c r="M47">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N47">
-        <v>-3.5</v>
-      </c>
-      <c r="O47">
-        <v>3.2</v>
-      </c>
-      <c r="P47">
-        <v>3.9</v>
-      </c>
-      <c r="Q47">
-        <v>3.6</v>
+      <c r="K47" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L47" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M47" s="3">
+        <v>4</v>
+      </c>
+      <c r="N47" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O47" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P47" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>3.9</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -5896,41 +5901,41 @@
         <v>582</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H48">
-        <v>-3.8</v>
-      </c>
-      <c r="I48">
-        <v>3.1</v>
-      </c>
-      <c r="J48">
-        <v>-6.5</v>
-      </c>
-      <c r="K48">
+        <v>119</v>
+      </c>
+      <c r="H48" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="I48" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="J48" s="3">
         <v>3.8</v>
       </c>
-      <c r="L48">
-        <v>-7.8</v>
-      </c>
-      <c r="M48">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N48">
-        <v>-3.5</v>
-      </c>
-      <c r="O48">
-        <v>3.2</v>
-      </c>
-      <c r="P48">
-        <v>3.9</v>
-      </c>
-      <c r="Q48">
-        <v>3.6</v>
+      <c r="K48" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L48" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="M48" s="3">
+        <v>4</v>
+      </c>
+      <c r="N48" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="O48" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="P48" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C48" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generate report for ARM
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB3B735-245C-4253-A0A4-35409909F387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A241B0-7EC4-406E-9ECA-27B76432FECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3355,10 +3355,10 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,34 +3497,26 @@
         <v>119</v>
       </c>
       <c r="H3" s="3">
-        <v>2.8</v>
+        <v>5</v>
       </c>
       <c r="I3" s="3">
-        <v>2.7</v>
-      </c>
-      <c r="J3" s="3">
-        <v>3.8</v>
-      </c>
-      <c r="K3" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="L3" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="M3" s="3">
-        <v>4</v>
-      </c>
+        <v>5.5</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="3">
-        <v>3.2</v>
+        <v>5.8</v>
       </c>
       <c r="O3" s="3">
-        <v>3.9</v>
+        <v>6.2</v>
       </c>
       <c r="P3" s="3">
-        <v>3.7</v>
+        <v>1.9</v>
       </c>
       <c r="Q3" s="3">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Generate report for INO
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A241B0-7EC4-406E-9ECA-27B76432FECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AFD208-6C15-41B7-BEEA-B8A4251C5AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3358,12 +3358,22 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -4008,34 +4018,30 @@
         <v>119</v>
       </c>
       <c r="H13" s="3">
-        <v>2.8</v>
+        <v>4.7</v>
       </c>
       <c r="I13" s="3">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="J13" s="3">
-        <v>3.8</v>
+        <v>6</v>
       </c>
       <c r="K13" s="3">
-        <v>3.2</v>
+        <v>4.5</v>
       </c>
       <c r="L13" s="3">
-        <v>4.2</v>
+        <v>6.4</v>
       </c>
       <c r="M13" s="3">
-        <v>4</v>
-      </c>
-      <c r="N13" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="O13" s="3">
-        <v>3.9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
       <c r="P13" s="3">
-        <v>3.7</v>
+        <v>1.4</v>
       </c>
       <c r="Q13" s="3">
-        <v>3.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -4116,34 +4122,34 @@
         <v>119</v>
       </c>
       <c r="H15" s="3">
-        <v>2.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I15" s="3">
-        <v>2.7</v>
+        <v>5.4</v>
       </c>
       <c r="J15" s="3">
-        <v>3.8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K15" s="3">
-        <v>3.2</v>
+        <v>5.6</v>
       </c>
       <c r="L15" s="3">
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="M15" s="3">
-        <v>4</v>
+        <v>6.3</v>
       </c>
       <c r="N15" s="3">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="O15" s="3">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
       <c r="P15" s="3">
-        <v>3.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Q15" s="3">
-        <v>3.9</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Generate report for IND
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\ADO-Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AFD208-6C15-41B7-BEEA-B8A4251C5AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4D8FFC-CE2A-4755-8F35-093C69A6C971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3358,7 +3358,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4068,34 +4068,34 @@
         <v>119</v>
       </c>
       <c r="H14" s="3">
-        <v>2.8</v>
+        <v>-8</v>
       </c>
       <c r="I14" s="3">
-        <v>2.7</v>
+        <v>10.3</v>
       </c>
       <c r="J14" s="3">
-        <v>3.8</v>
+        <v>-10</v>
       </c>
       <c r="K14" s="3">
-        <v>3.2</v>
+        <v>11.4</v>
       </c>
       <c r="L14" s="3">
-        <v>4.2</v>
+        <v>-15.7</v>
       </c>
       <c r="M14" s="3">
-        <v>4</v>
+        <v>15.2</v>
       </c>
       <c r="N14" s="3">
-        <v>3.2</v>
+        <v>-9.9</v>
       </c>
       <c r="O14" s="3">
-        <v>3.9</v>
+        <v>12.5</v>
       </c>
       <c r="P14" s="3">
-        <v>3.7</v>
+        <v>6.3</v>
       </c>
       <c r="Q14" s="3">
-        <v>3.9</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>